<commit_message>
add new eindkomst endpoint
</commit_message>
<xml_diff>
--- a/app/background_on_endpoints/prod_services.xlsx
+++ b/app/background_on_endpoints/prod_services.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diverse_projekter\serviceplatformen\app\background_on_endpoints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev_ops_projekter\serviceplatformen_python\app\background_on_endpoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F25A63D-C19A-4354-919F-1E38FCE4CA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D68238A-2A54-433A-94A7-5EAA136554FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{55EBC655-7FD9-4733-9DCE-57215F606CC4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55EBC655-7FD9-4733-9DCE-57215F606CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>PersonLookup</t>
   </si>
   <si>
-    <t>IndkomstoplysningerLaes</t>
-  </si>
-  <si>
     <t>EffektueringHentUDKKommune</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>http://serviceplatformen.dk/xml/wsdl/soap11/CPR/PersonBaseDataExtended/5/PersonLookup</t>
   </si>
   <si>
-    <t>http://serviceplatformen.dk/xml/wsdl/soap11/SKAT/EIndkomst/3/IndkomstoplysningerLaes</t>
-  </si>
-  <si>
     <t>http://serviceplatformen.dk/xml/wsdl/soap11/SP/Demo/1/callDemoService</t>
   </si>
   <si>
@@ -158,15 +152,9 @@
     <t>http://demo.prod-serviceplatformen.dk/service/DemoService/2</t>
   </si>
   <si>
-    <t>http://skat.serviceplatformen.dk/service/eindkomst/3</t>
-  </si>
-  <si>
     <t>https://prod.serviceplatformen.dk/service/SP/Demo/2</t>
   </si>
   <si>
-    <t>https://prod.serviceplatformen.dk/service/SKAT/EIndkomst/3</t>
-  </si>
-  <si>
     <t>https://saml.adgangsstyring.stoettesystemerne.dk</t>
   </si>
   <si>
@@ -174,6 +162,18 @@
   </si>
   <si>
     <t>callDemoService</t>
+  </si>
+  <si>
+    <t>http://entityid.kombit.dk/service/sp/skatforwardeindkomstservice/4</t>
+  </si>
+  <si>
+    <t>http://www.kombit.dk/2017/01/01/SKATForwardEIndkomstServiceService_4#SF0770_A_IndkomstoplysningerLaes_IndkomstoplysningerLaes</t>
+  </si>
+  <si>
+    <t>SF0770_A_IndkomstoplysningerLaes_IndkomstoplysningerLaes</t>
+  </si>
+  <si>
+    <t>https://prod.serviceplatformen.dk/service/SKAT/EIndkomst/4</t>
   </si>
 </sst>
 </file>
@@ -274,9 +274,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 Tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -314,7 +314,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -420,7 +420,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -562,7 +562,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -573,25 +573,25 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.7265625" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="89.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.81640625" customWidth="1"/>
-    <col min="11" max="11" width="76.453125" customWidth="1"/>
+    <col min="1" max="1" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="89.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.85546875" customWidth="1"/>
+    <col min="11" max="11" width="76.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -626,30 +626,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>11</v>
@@ -661,30 +661,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>11</v>
@@ -696,30 +696,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>11</v>
@@ -731,30 +731,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>11</v>
@@ -766,30 +766,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>14</v>
@@ -802,25 +802,27 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{CA2B8FED-677B-4925-AB7D-6F4675AC0056}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{687150E8-72A2-4BF6-93E9-3B9ABCFC930D}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{11B0FC1E-3093-4A36-9281-663D8EAE2FE8}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{3A251E57-5E57-47BC-9C6B-26ABF2EC8850}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{FFE13638-793B-46E6-9736-31B05525FE48}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{A576CC9D-DC16-44D0-8FC1-6B6E2EC4E404}"/>
-    <hyperlink ref="G3:G5" r:id="rId7" display="https://adgangsstyring.stoettesystemerne.dk/runtime/services/kombittrust/14/certificatemixed" xr:uid="{4390476D-E08A-4630-B9C8-7B5999C49B11}"/>
-    <hyperlink ref="G6" r:id="rId8" xr:uid="{18B49173-0733-4BF6-8A79-020EC49A5ED8}"/>
-    <hyperlink ref="H2" r:id="rId9" display="https://adgangsstyring.stoettesystemerne.dk" xr:uid="{612234D0-734A-43DB-B5BD-F5C06DD0225E}"/>
-    <hyperlink ref="H3:H5" r:id="rId10" display="https://adgangsstyring.stoettesystemerne.dk" xr:uid="{FBBF5F88-AA6D-4D76-B130-E6C26458D797}"/>
-    <hyperlink ref="E2" r:id="rId11" xr:uid="{D87AB230-2227-4AE4-91F8-9F345A0D48FB}"/>
-    <hyperlink ref="E3" r:id="rId12" xr:uid="{23E1C6AE-DF30-4F72-A1D4-05CEF58EF4D0}"/>
-    <hyperlink ref="A3" r:id="rId13" xr:uid="{A3BC0650-99A8-4CD5-BC59-63D1985041CD}"/>
-    <hyperlink ref="A2" r:id="rId14" xr:uid="{A06D63AB-682F-4AB8-A058-32F8A1DD44CD}"/>
-    <hyperlink ref="A4" r:id="rId15" xr:uid="{9814685A-A983-4109-8658-B16D2B23AD1C}"/>
-    <hyperlink ref="A6" r:id="rId16" xr:uid="{A15C5C8C-4226-43B3-A8B4-D7B72E3078AB}"/>
-    <hyperlink ref="E6" r:id="rId17" xr:uid="{DA53C8A8-706C-455D-B036-5A926F71B652}"/>
-    <hyperlink ref="A5" r:id="rId18" display="http://demo.prod-serviceplatformen.dk/service/DemoService/1" xr:uid="{3F3F8A31-179C-4C3F-84C0-08CB05BA8B8D}"/>
-    <hyperlink ref="E4" r:id="rId19" xr:uid="{61FC2021-7C84-4426-867F-E8DB31228DCA}"/>
-    <hyperlink ref="E5" r:id="rId20" display="https://prod.serviceplatformen.dk/service/SP/Demo/1 " xr:uid="{D682C3C6-6FBD-4ABE-8612-CA91E3718395}"/>
-    <hyperlink ref="H6" r:id="rId21" display="https://adgangsstyring.stoettesystemerne.dk" xr:uid="{F69DF5D5-2F01-4D35-8E86-1C8A31365C80}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{3A251E57-5E57-47BC-9C6B-26ABF2EC8850}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{FFE13638-793B-46E6-9736-31B05525FE48}"/>
+    <hyperlink ref="G2" r:id="rId5" xr:uid="{A576CC9D-DC16-44D0-8FC1-6B6E2EC4E404}"/>
+    <hyperlink ref="G3:G5" r:id="rId6" display="https://adgangsstyring.stoettesystemerne.dk/runtime/services/kombittrust/14/certificatemixed" xr:uid="{4390476D-E08A-4630-B9C8-7B5999C49B11}"/>
+    <hyperlink ref="G6" r:id="rId7" xr:uid="{18B49173-0733-4BF6-8A79-020EC49A5ED8}"/>
+    <hyperlink ref="H2" r:id="rId8" display="https://adgangsstyring.stoettesystemerne.dk" xr:uid="{612234D0-734A-43DB-B5BD-F5C06DD0225E}"/>
+    <hyperlink ref="H3:H5" r:id="rId9" display="https://adgangsstyring.stoettesystemerne.dk" xr:uid="{FBBF5F88-AA6D-4D76-B130-E6C26458D797}"/>
+    <hyperlink ref="E2" r:id="rId10" xr:uid="{D87AB230-2227-4AE4-91F8-9F345A0D48FB}"/>
+    <hyperlink ref="E3" r:id="rId11" xr:uid="{23E1C6AE-DF30-4F72-A1D4-05CEF58EF4D0}"/>
+    <hyperlink ref="A3" r:id="rId12" xr:uid="{A3BC0650-99A8-4CD5-BC59-63D1985041CD}"/>
+    <hyperlink ref="A2" r:id="rId13" xr:uid="{A06D63AB-682F-4AB8-A058-32F8A1DD44CD}"/>
+    <hyperlink ref="A6" r:id="rId14" xr:uid="{A15C5C8C-4226-43B3-A8B4-D7B72E3078AB}"/>
+    <hyperlink ref="E6" r:id="rId15" xr:uid="{DA53C8A8-706C-455D-B036-5A926F71B652}"/>
+    <hyperlink ref="A5" r:id="rId16" display="http://demo.prod-serviceplatformen.dk/service/DemoService/1" xr:uid="{3F3F8A31-179C-4C3F-84C0-08CB05BA8B8D}"/>
+    <hyperlink ref="E5" r:id="rId17" display="https://prod.serviceplatformen.dk/service/SP/Demo/1 " xr:uid="{D682C3C6-6FBD-4ABE-8612-CA91E3718395}"/>
+    <hyperlink ref="H6" r:id="rId18" display="https://adgangsstyring.stoettesystemerne.dk" xr:uid="{F69DF5D5-2F01-4D35-8E86-1C8A31365C80}"/>
+    <hyperlink ref="G4" r:id="rId19" xr:uid="{74B0C382-69AB-4DBD-A89C-0E4D1F11D829}"/>
+    <hyperlink ref="H4" r:id="rId20" display="https://adgangsstyring.stoettesystemerne.dk" xr:uid="{8E8A27D2-6D11-443F-A3EC-1314FF67DEF0}"/>
+    <hyperlink ref="E4" r:id="rId21" xr:uid="{5DF01244-AEDC-44ED-A645-CCE7128328E0}"/>
+    <hyperlink ref="A4" r:id="rId22" xr:uid="{09796036-2F07-40A7-9E9A-DE990D115B9D}"/>
+    <hyperlink ref="B4" r:id="rId23" location="SF0770_A_IndkomstoplysningerLaes_IndkomstoplysningerLaes" xr:uid="{65414C58-6B48-4BF5-A644-2BFB1E5C49C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>